<commit_message>
add clean architecture pattern
</commit_message>
<xml_diff>
--- a/VorodKhoroj/Resources/holiday.xlsx
+++ b/VorodKhoroj/Resources/holiday.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Github\VorodKhoroj\VorodKhoroj\bin\Debug\net8.0-windows\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Project\aliansari685\VorodKhoroj\VorodKhoroj\bin\Debug\net8.0-windows\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD5CD689-2DF3-4772-A690-23FA401F324B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0555081-5F2D-4611-AFBF-8C543A7192F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{E8CDD0C3-C3C7-4750-9482-C94288EF7135}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{E8CDD0C3-C3C7-4750-9482-C94288EF7135}"/>
   </bookViews>
   <sheets>
     <sheet name="Holiday" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>Title</t>
   </si>
@@ -53,9 +53,30 @@
     <t>Date</t>
   </si>
   <si>
+    <t>عید سعید باستان</t>
+  </si>
+  <si>
+    <t>1403/01/01</t>
+  </si>
+  <si>
+    <t>1403/01/02</t>
+  </si>
+  <si>
+    <t>1403/01/03</t>
+  </si>
+  <si>
+    <t>1403/01/04</t>
+  </si>
+  <si>
     <t>تعطیل</t>
   </si>
   <si>
+    <t>1403/01/12</t>
+  </si>
+  <si>
+    <t>1403/01/13</t>
+  </si>
+  <si>
     <t>1403/01/22</t>
   </si>
   <si>
@@ -114,9 +135,6 @@
   </si>
   <si>
     <t>1403/11/22</t>
-  </si>
-  <si>
-    <t>1403/12/29</t>
   </si>
   <si>
     <t>روز کارگر</t>
@@ -213,7 +231,7 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{03C3DFE2-388C-47ED-9985-CFFDB8D1F4B6}" name="Holiday_1" displayName="Holiday_1" ref="A1:B79" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B79" xr:uid="{03C3DFE2-388C-47ED-9985-CFFDB8D1F4B6}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B28">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B79">
     <sortCondition ref="B1:B79"/>
   </sortState>
   <tableColumns count="2">
@@ -521,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D249172-7200-4C77-B49D-94403AE10118}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,15 +577,15 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -575,87 +593,87 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
         <v>17</v>
@@ -663,7 +681,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -671,7 +689,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
@@ -679,34 +697,74 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>7</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>